<commit_message>
Updated shape and dtype formatting for h5getInfo
Escape ',' in field names of compound types.
</commit_message>
<xml_diff>
--- a/test/xlsx/h5getInfo.xlsx
+++ b/test/xlsx/h5getInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>Shape:</t>
   </si>
   <si>
-    <t>(721, 841)</t>
-  </si>
-  <si>
     <t>Type:</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>C:\Users\Gerd\git\PyHexad\test\xlsx\</t>
+  </si>
+  <si>
+    <t>{ 721, 841 }</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -728,15 +730,15 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>